<commit_message>
Added ImageReg testing arenas
Arenas are reflected in the excel file :
- 1i.txt and 2i.txt for basic testing
- 3i.txt for staircase testing
</commit_message>
<xml_diff>
--- a/Algorithms/src/logic/exploration/BlkSurface_Visualization.xlsx
+++ b/Algorithms/src/logic/exploration/BlkSurface_Visualization.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilso\Desktop\MDP-Autonomous-Robot-Grp-33\Algorithms\src\logic\exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8C674B-5F66-4BAE-995E-FCC9DABB92CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7AD4FE-69B4-42A8-A1B5-BF90E40ADE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{286CAD39-EDF2-4F39-BD97-BFAC0DBCBC30}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" activeTab="2" xr2:uid="{286CAD39-EDF2-4F39-BD97-BFAC0DBCBC30}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic1" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic2" sheetId="3" r:id="rId2"/>
+    <sheet name="Staircase" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>64S</t>
   </si>
@@ -83,16 +85,124 @@
     <t>28S</t>
   </si>
   <si>
-    <t>37W</t>
-  </si>
-  <si>
-    <t>17E</t>
-  </si>
-  <si>
     <t>26N</t>
   </si>
   <si>
     <t>13|18</t>
+  </si>
+  <si>
+    <t>3|7</t>
+  </si>
+  <si>
+    <t>0|7</t>
+  </si>
+  <si>
+    <t>0|6</t>
+  </si>
+  <si>
+    <t>0|5</t>
+  </si>
+  <si>
+    <t>0|4</t>
+  </si>
+  <si>
+    <t>1|7</t>
+  </si>
+  <si>
+    <t>47W</t>
+  </si>
+  <si>
+    <t>18S</t>
+  </si>
+  <si>
+    <t>38S</t>
+  </si>
+  <si>
+    <t>06N</t>
+  </si>
+  <si>
+    <t>03N</t>
+  </si>
+  <si>
+    <t>08S</t>
+  </si>
+  <si>
+    <t>16N</t>
+  </si>
+  <si>
+    <t>36N</t>
+  </si>
+  <si>
+    <t>5|0</t>
+  </si>
+  <si>
+    <t>7|2</t>
+  </si>
+  <si>
+    <t>8|3</t>
+  </si>
+  <si>
+    <t>84S</t>
+  </si>
+  <si>
+    <t>93W</t>
+  </si>
+  <si>
+    <t>51S</t>
+  </si>
+  <si>
+    <t>71S</t>
+  </si>
+  <si>
+    <t>51SE</t>
+  </si>
+  <si>
+    <t>73SE</t>
+  </si>
+  <si>
+    <t>62SE</t>
+  </si>
+  <si>
+    <t>82NW</t>
+  </si>
+  <si>
+    <t>60NW</t>
+  </si>
+  <si>
+    <t>71NW</t>
+  </si>
+  <si>
+    <t>40E</t>
+  </si>
+  <si>
+    <t>16W</t>
+  </si>
+  <si>
+    <t>15W</t>
+  </si>
+  <si>
+    <t>14W</t>
+  </si>
+  <si>
+    <t>17W</t>
+  </si>
+  <si>
+    <t>7|0</t>
+  </si>
+  <si>
+    <t>4|0</t>
+  </si>
+  <si>
+    <t>61S</t>
+  </si>
+  <si>
+    <t>41S</t>
+  </si>
+  <si>
+    <t>30E</t>
+  </si>
+  <si>
+    <t>80W</t>
   </si>
 </sst>
 </file>
@@ -507,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0AD0FE-46AB-4C2D-B84A-BEF8E5180B61}">
   <dimension ref="C2:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -554,7 +664,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="R3" s="3"/>
     </row>
@@ -742,12 +852,18 @@
       <c r="C13" s="1">
         <v>8</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -764,17 +880,21 @@
       <c r="C14" s="1">
         <v>7</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>17</v>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="2"/>
+      <c r="G14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -790,12 +910,18 @@
       <c r="C15" s="1">
         <v>6</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -838,9 +964,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -859,15 +983,9 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -885,15 +1003,9 @@
       <c r="F19" s="5"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -912,15 +1024,17 @@
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="I20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>12</v>
+        <v>37</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -937,6 +1051,527 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
+      <c r="G21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>5</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6</v>
+      </c>
+      <c r="K22" s="1">
+        <v>7</v>
+      </c>
+      <c r="L22" s="1">
+        <v>8</v>
+      </c>
+      <c r="M22" s="1">
+        <v>9</v>
+      </c>
+      <c r="N22" s="1">
+        <v>10</v>
+      </c>
+      <c r="O22" s="1">
+        <v>11</v>
+      </c>
+      <c r="P22" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>13</v>
+      </c>
+      <c r="R22" s="1">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7F6C46-C32C-4085-8C0D-9C76C84C6234}">
+  <dimension ref="C2:R22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="16384" width="4.41015625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="1">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="1">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="1">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C8" s="1">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="1">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
@@ -1006,4 +1641,525 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6630C822-1917-4234-B708-1830113AF5CA}">
+  <dimension ref="C2:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="16384" width="4.41015625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="1">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="1">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="1">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C8" s="1">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="1">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>5</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6</v>
+      </c>
+      <c r="K22" s="1">
+        <v>7</v>
+      </c>
+      <c r="L22" s="1">
+        <v>8</v>
+      </c>
+      <c r="M22" s="1">
+        <v>9</v>
+      </c>
+      <c r="N22" s="1">
+        <v>10</v>
+      </c>
+      <c r="O22" s="1">
+        <v>11</v>
+      </c>
+      <c r="P22" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>13</v>
+      </c>
+      <c r="R22" s="1">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add 4i.txt - tricky image reg arena
</commit_message>
<xml_diff>
--- a/Algorithms/src/logic/exploration/BlkSurface_Visualization.xlsx
+++ b/Algorithms/src/logic/exploration/BlkSurface_Visualization.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilso\Desktop\MDP-Autonomous-Robot-Grp-33\Algorithms\src\logic\exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7AD4FE-69B4-42A8-A1B5-BF90E40ADE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1007DC9-ACE3-4C80-A5BE-82D60236F995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" activeTab="2" xr2:uid="{286CAD39-EDF2-4F39-BD97-BFAC0DBCBC30}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" activeTab="3" xr2:uid="{286CAD39-EDF2-4F39-BD97-BFAC0DBCBC30}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic1" sheetId="1" r:id="rId1"/>
     <sheet name="Basic2" sheetId="3" r:id="rId2"/>
     <sheet name="Staircase" sheetId="2" r:id="rId3"/>
+    <sheet name="Tricky" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>64S</t>
   </si>
@@ -203,13 +204,49 @@
   </si>
   <si>
     <t>80W</t>
+  </si>
+  <si>
+    <t>73SEW</t>
+  </si>
+  <si>
+    <t>62NE</t>
+  </si>
+  <si>
+    <t>71N</t>
+  </si>
+  <si>
+    <t>4|8</t>
+  </si>
+  <si>
+    <t>5|7</t>
+  </si>
+  <si>
+    <t>56N</t>
+  </si>
+  <si>
+    <t>47NWE</t>
+  </si>
+  <si>
+    <t>27E</t>
+  </si>
+  <si>
+    <t>67W</t>
+  </si>
+  <si>
+    <t>49S</t>
+  </si>
+  <si>
+    <t>38SE</t>
+  </si>
+  <si>
+    <t>58SW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +256,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -284,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,6 +343,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0AD0FE-46AB-4C2D-B84A-BEF8E5180B61}">
   <dimension ref="C2:R22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1133,7 +1192,7 @@
   <dimension ref="C2:R22"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:K21"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1647,11 +1706,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6630C822-1917-4234-B708-1830113AF5CA}">
   <dimension ref="C2:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="11.7" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="16384" width="4.41015625" style="1"/>
   </cols>
@@ -2162,4 +2221,517 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF5593F-578B-4272-ADDE-955A94C6634F}">
+  <dimension ref="C2:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="123" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.41015625" defaultRowHeight="10" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="16384" width="4.41015625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="6">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+    </row>
+    <row r="3" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="6">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="8"/>
+    </row>
+    <row r="4" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="6">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+    </row>
+    <row r="5" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="6">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+    </row>
+    <row r="7" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="6">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C8" s="6">
+        <v>13</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="6">
+        <v>12</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="6">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="6">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C12" s="6">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="6">
+        <v>8</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+    </row>
+    <row r="14" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="6">
+        <v>7</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C15" s="6">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+    </row>
+    <row r="16" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C16" s="6">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="6">
+        <v>4</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+    </row>
+    <row r="18" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C18" s="6">
+        <v>3</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+    </row>
+    <row r="20" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+    </row>
+    <row r="21" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+    </row>
+    <row r="22" spans="3:18" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2</v>
+      </c>
+      <c r="G22" s="6">
+        <v>3</v>
+      </c>
+      <c r="H22" s="6">
+        <v>4</v>
+      </c>
+      <c r="I22" s="6">
+        <v>5</v>
+      </c>
+      <c r="J22" s="6">
+        <v>6</v>
+      </c>
+      <c r="K22" s="6">
+        <v>7</v>
+      </c>
+      <c r="L22" s="6">
+        <v>8</v>
+      </c>
+      <c r="M22" s="6">
+        <v>9</v>
+      </c>
+      <c r="N22" s="6">
+        <v>10</v>
+      </c>
+      <c r="O22" s="6">
+        <v>11</v>
+      </c>
+      <c r="P22" s="6">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>13</v>
+      </c>
+      <c r="R22" s="6">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>